<commit_message>
add info on shared code
</commit_message>
<xml_diff>
--- a/2018_2019/Misc/HalloweenPumpkins/IEP20182019.xlsx
+++ b/2018_2019/Misc/HalloweenPumpkins/IEP20182019.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esther\Documents\Research\HalloweenPumpkins\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esther\Documents\GitHub\instruments-master\2018_2019\Misc\HalloweenPumpkins\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="27870" windowHeight="11685"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="11685"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -613,9 +613,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000000"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -670,8 +669,8 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -980,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,7 +1040,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="5">
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1104,7 +1103,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="5">
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1628,6 +1627,9 @@
       <c r="D43" t="s">
         <v>3</v>
       </c>
+      <c r="E43" s="5">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -1986,11 +1988,14 @@
       <c r="D67" t="s">
         <v>3</v>
       </c>
+      <c r="E67" s="5">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E68" s="5">
         <f>SUM(E3:E67)</f>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some pumpkins with 40 minutes to go
</commit_message>
<xml_diff>
--- a/2018_2019/Misc/HalloweenPumpkins/IEP20182019.xlsx
+++ b/2018_2019/Misc/HalloweenPumpkins/IEP20182019.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="11685"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="27870" windowHeight="11685"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -979,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,11 +1345,14 @@
       <c r="B24" t="s">
         <v>128</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>129</v>
       </c>
       <c r="D24" t="s">
         <v>3</v>
+      </c>
+      <c r="E24" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1393,11 +1396,14 @@
       <c r="B27" t="s">
         <v>43</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D27" t="s">
         <v>3</v>
+      </c>
+      <c r="E27" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1856,11 +1862,14 @@
       <c r="B58" t="s">
         <v>190</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="2" t="s">
         <v>191</v>
       </c>
       <c r="D58" t="s">
         <v>3</v>
+      </c>
+      <c r="E58" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1915,11 +1924,14 @@
       <c r="B62" t="s">
         <v>131</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="2" t="s">
         <v>132</v>
       </c>
       <c r="D62" t="s">
         <v>3</v>
+      </c>
+      <c r="E62" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2007,7 +2019,7 @@
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E68" s="5">
         <f>SUM(E3:E67)</f>
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2033,6 +2045,10 @@
     <hyperlink ref="C14" r:id="rId15"/>
     <hyperlink ref="C45" r:id="rId16"/>
     <hyperlink ref="C16" r:id="rId17"/>
+    <hyperlink ref="C62" r:id="rId18"/>
+    <hyperlink ref="C58" r:id="rId19"/>
+    <hyperlink ref="C27" r:id="rId20"/>
+    <hyperlink ref="C24" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>